<commit_message>
Obtener Datos de un PDF pasarlo a Excel
</commit_message>
<xml_diff>
--- a/Buscar_cuarto/Buscar_cuarto/Resultados.xlsx
+++ b/Buscar_cuarto/Buscar_cuarto/Resultados.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="267">
   <si>
     <t>Nombre</t>
   </si>
@@ -54,387 +54,12 @@
     <t>Excelente</t>
   </si>
   <si>
-    <t>AC Hotel Guadalajara México</t>
-  </si>
-  <si>
-    <t>Moderno hotel de negocios con una vistosa arquitectura, piscina climatizada tipo infinity, gimnasio, WiFi en cortesía, salones de eventos y 188 cuartos con ventanales panorámicos.</t>
-  </si>
-  <si>
-    <t>MXN$ 11,641</t>
-  </si>
-  <si>
     <t>Guadalajara</t>
   </si>
   <si>
-    <t>Aranzazú Centro Histórico Guadalajara</t>
-  </si>
-  <si>
-    <t>Céntrico y totalmente acondicionado con salones para eventos, este hotel es perfecto para los negocios.</t>
-  </si>
-  <si>
-    <t>MXN$ 4,674</t>
-  </si>
-  <si>
-    <t>Aranzazú Eco</t>
-  </si>
-  <si>
-    <t>Con una envidiable locación y prácticos servicios, esta propiedad es magnfífica para tu estadía.</t>
-  </si>
-  <si>
-    <t>MXN$ 4,048</t>
-  </si>
-  <si>
-    <t>Arboledas Expo</t>
-  </si>
-  <si>
-    <t>Si buscas comodidad y conveniencia en tu visita por la ciudad, considera este hotel como una buena opción.</t>
-  </si>
-  <si>
-    <t>MXN$ 3,640</t>
-  </si>
-  <si>
-    <t>Aurea Hotel and Suites</t>
-  </si>
-  <si>
-    <t>Hotel ideal para largas estadías en el suroeste de la ciudad, con fácil acceso a la Plaza del Sol. Tiene suites con cocineta, una piscina y amplio jardín. Acepta mascotas.</t>
-  </si>
-  <si>
-    <t>MXN$ 5,906</t>
-  </si>
-  <si>
     <t>Zapopan</t>
   </si>
   <si>
-    <t>Best Western Plus Gran Hotel Centro Histórico Guadalajara</t>
-  </si>
-  <si>
-    <t>Céntrico hotel frente a una plaza comercial y a 16 km del aeropuerto, con salones de eventos y más.</t>
-  </si>
-  <si>
-    <t>MXN$ 4,750</t>
-  </si>
-  <si>
-    <t>Camino Real Guadalajara</t>
-  </si>
-  <si>
-    <t>Este hotel cuenta con un servicio de primer mundo para una experiencia única e inolvidable.</t>
-  </si>
-  <si>
-    <t>MXN$ 8,398</t>
-  </si>
-  <si>
-    <t>Casa Monraz Hotel Boutique and Galeria</t>
-  </si>
-  <si>
-    <t>Hotel boutique de arquitectura francesa en una zona cercana al centro histórico. Decorado con obras de arte, ofrece restaurante, bar de tapas, servicios de negocios y hermosos cuartos.</t>
-  </si>
-  <si>
-    <t>MXN$ 10,409</t>
-  </si>
-  <si>
-    <t>City Express Guadalajara Aeropuerto</t>
-  </si>
-  <si>
-    <t>Hotel de negocios al sur de la ciudad, ofrece desayuno en cortesía y se ubica a unos cuantos minutos del aeropuerto internacional.</t>
-  </si>
-  <si>
-    <t>MXN$ 6,879</t>
-  </si>
-  <si>
-    <t>City Express Junior Guadalajara Periférico Sur</t>
-  </si>
-  <si>
-    <t>Excelentes servcios y amenidades, así como una increíble ubicación a precios competitivos.</t>
-  </si>
-  <si>
-    <t>MXN$ 4,894</t>
-  </si>
-  <si>
-    <t>Tlaquepaque</t>
-  </si>
-  <si>
-    <t>City Express Plus Guadalajara Expo</t>
-  </si>
-  <si>
-    <t>Hotel de negocios a 6 cuadras del centro de convenciones Expo Guadalajara y a pasos del centro comercial Plaza del Sol. Ofrece sala de juntas, Wi-Fi y gimnasio.</t>
-  </si>
-  <si>
-    <t>MXN$ 7,207</t>
-  </si>
-  <si>
-    <t>City Express Plus Guadalajara Palomar</t>
-  </si>
-  <si>
-    <t>Un hotel en la zona de Palomar con modernas habitaciones, WiFi, desayuno, centro de negocios y salas de juntas.</t>
-  </si>
-  <si>
-    <t>MXN$ 7,175</t>
-  </si>
-  <si>
-    <t>City Express Tepatitlán</t>
-  </si>
-  <si>
-    <t>Hotel de negocios, con prácticas instalaciones equipadas con gimnasio, sala de juntas y desayunador entre otros para tu comodidad.</t>
-  </si>
-  <si>
-    <t>MXN$ 5,267</t>
-  </si>
-  <si>
-    <t>Country Plaza</t>
-  </si>
-  <si>
-    <t>Las fantásticas instalaciones de este hotel satisfacen al ejecutivo y al turista por igual.</t>
-  </si>
-  <si>
-    <t>MXN$ 6,548</t>
-  </si>
-  <si>
-    <t>El Tapatío Hotel and Resort</t>
-  </si>
-  <si>
-    <t>Vive unas vacaciones rodeado de todas las comodidades y disfruta al máximo las bellas instalaciones de esta propiedad colonial</t>
-  </si>
-  <si>
-    <t>MXN$ 12,834</t>
-  </si>
-  <si>
-    <t>Encore Hotel Guadalajara</t>
-  </si>
-  <si>
-    <t>Moderno hotel de negocios con un vanguardista diseño, gimnasio con vista panorámica, salones, bar con juegos de mesa y habitaciones con sofisticados servicios.</t>
-  </si>
-  <si>
-    <t>MXN$ 9,102</t>
-  </si>
-  <si>
-    <t>European Life Style Executive Suites</t>
-  </si>
-  <si>
-    <t>Hotel que cuenta con suites tipo departamento perfectamente equipadas para largas estancias y para familias o grupos de amigos en viaje de negocios o placer.</t>
-  </si>
-  <si>
-    <t>MXN$ 3,232</t>
-  </si>
-  <si>
-    <t>Expohotel</t>
-  </si>
-  <si>
-    <t>Sencilla propiedad con acceso a Internet inalámbrico, llamadas locales en cortesía y cuartos climatizados. Está frente al WTC y cerca de Expo Guadalajara.</t>
-  </si>
-  <si>
-    <t>MXN$ 2,245</t>
-  </si>
-  <si>
-    <t>FCH Hotel Expo - Adults Only</t>
-  </si>
-  <si>
-    <t>Hotel boutique en un Residencial a 42 minutos del aeropuerto, con habitaciones bien equipadas y restaurante.</t>
-  </si>
-  <si>
-    <t>MXN$ 6,725</t>
-  </si>
-  <si>
-    <t>Fiesta Americana Guadalajara</t>
-  </si>
-  <si>
-    <t>El lugar favorito de los viajeros que buscan alojamiento de primera clase en la capital de Jalisco, por su ubicación, servicio e instalaciones.</t>
-  </si>
-  <si>
-    <t>MXN$ 11,638</t>
-  </si>
-  <si>
-    <t>Fiesta Inn Guadalajara Expo</t>
-  </si>
-  <si>
-    <t>Hotel de negocios, a 22.5 km del aeropuerto, a 5 minutos de la Expo Guadalajara y del shopping Plaza del Sol.</t>
-  </si>
-  <si>
-    <t>MXN$ 8,007</t>
-  </si>
-  <si>
-    <t>Grand Fiesta Americana Guadalajara Country Club</t>
-  </si>
-  <si>
-    <t>Aquí encontrarás magníficos centros de consumo, un completo spa, gimnasio con vista panorámica y mucho más</t>
-  </si>
-  <si>
-    <t>MXN$ 12,838</t>
-  </si>
-  <si>
-    <t>Guadalajara Plaza Ejecutivo López Mateos</t>
-  </si>
-  <si>
-    <t>Hotel de negocios en un importante distrito comercial, con cuartos cómodos, a 25 km del aeropuerto.</t>
-  </si>
-  <si>
-    <t>MXN$ 5,534</t>
-  </si>
-  <si>
-    <t>Guadalajara Plaza Expo Business Class</t>
-  </si>
-  <si>
-    <t>Moderna propiedad con acogedoras habitaciones, restaurante, áreas para eventos y la tradicional hospitalidad tapatía</t>
-  </si>
-  <si>
-    <t>MXN$ 6,345</t>
-  </si>
-  <si>
-    <t>Hacienda Sepúlveda Hotel and Spa</t>
-  </si>
-  <si>
-    <t>Romántico hotel boutique con spa, lago propio, actividades, restaurante, bar, piscina, jacuzzi rodeado de jardines y habitaciones decoradas en estilo colonial.</t>
-  </si>
-  <si>
-    <t>MXN$ 12,920</t>
-  </si>
-  <si>
-    <t>Lagos de Moreno</t>
-  </si>
-  <si>
-    <t>Hampton Inn by Hilton Guadalajara Expo</t>
-  </si>
-  <si>
-    <t>Conveniente ubicación a 3 cuadras de Expo Guadalajara, con centro de negocios, salón de eventos, bar, desayunador, estacionamiento, gimnasio y finas habitaciones.</t>
-  </si>
-  <si>
-    <t>MXN$ 8,926</t>
-  </si>
-  <si>
-    <t>Hampton Inn Guadalajara Aeropuerto</t>
-  </si>
-  <si>
-    <t>Hotel de negocios con fácil acceso al aeropuerto. Tiene piscina al aire libre, gimnasio, centro de negocios 24 horas, servicio de transportación e Internet en todas las áreas.</t>
-  </si>
-  <si>
-    <t>MXN$ 9,860</t>
-  </si>
-  <si>
-    <t>HG Hotel</t>
-  </si>
-  <si>
-    <t>Si buscas alta calidad en el servicio y excelente precio, este hotel es el sitio ideal.</t>
-  </si>
-  <si>
-    <t>MXN$ 8,832</t>
-  </si>
-  <si>
-    <t>Hilton Guadalajara</t>
-  </si>
-  <si>
-    <t>Hotel de negocios con servicios de spa, piscina, restaurantes, bar y gimnasio, a 28 km del Aeropuerto Internacional de Guadalajara Miguel Hidalgo y Costilla.</t>
-  </si>
-  <si>
-    <t>MXN$ 7,304</t>
-  </si>
-  <si>
-    <t>Holiday Inn Centro Histórico Guadalajara</t>
-  </si>
-  <si>
-    <t>Un hotel con todo lo que necesitas para una satisfactoria estancia de negocios o de vacaciones en el centro histórico de Guadalajara</t>
-  </si>
-  <si>
-    <t>MXN$ 7,531</t>
-  </si>
-  <si>
-    <t>Holiday Inn Express Guadalajara Expo</t>
-  </si>
-  <si>
-    <t>Hotel de negocios cerca del centro comercial Plaza del Sol y del centro de convenciones Expo Guadalajara. Tiene piscina exterior y una vistosa fachada de cristal.</t>
-  </si>
-  <si>
-    <t>MXN$ 8,621</t>
-  </si>
-  <si>
-    <t>Holiday Inn Express Guadalajara UAG</t>
-  </si>
-  <si>
-    <t>Hotel de negocios con una vistosa arquitectura, piscina, estacionamiento y acceso a Internet inalámbrico. Situado junto a la Universidad Autónoma de Guadalajara.</t>
-  </si>
-  <si>
-    <t>MXN$ 9,024</t>
-  </si>
-  <si>
-    <t>Holiday Inn Guadalajara Expo</t>
-  </si>
-  <si>
-    <t>Aquí encontrarás lujo, confort y las más completas amenidades y servicios para los altos ejecutivos en viaje de negocios.</t>
-  </si>
-  <si>
-    <t>MXN$ 8,227</t>
-  </si>
-  <si>
-    <t>Holiday Inn Guadalajara Select</t>
-  </si>
-  <si>
-    <t>Un hotel de negocios con una cálida atención y todo lo necesario para el viajero por cuestiones de trabajo</t>
-  </si>
-  <si>
-    <t>MXN$ 8,619</t>
-  </si>
-  <si>
-    <t>Hostalia Hotel Expo &amp; Business Class</t>
-  </si>
-  <si>
-    <t>Moderno y bien equipado hotel de negocios con restaurante, bar, gimnasio e instalaciones para eventos y conferencias en una importante avenida de la ciudad.</t>
-  </si>
-  <si>
-    <t>MXN$ 5,566</t>
-  </si>
-  <si>
-    <t>Hotel Alcázar</t>
-  </si>
-  <si>
-    <t>Céntrico hotel sobre una importante avenida, a unas cuadras de la catedral. Tiene restaurante, Wi-Fi, centro de negocios y cuartos insonorizados con piso de madera.</t>
-  </si>
-  <si>
-    <t>MXN$ 3,141</t>
-  </si>
-  <si>
-    <t>Hotel and Suites Quinta Magna</t>
-  </si>
-  <si>
-    <t>Hotel de negocios cercano a lugares de interés turístico, oficinas y tres plazas comerciales. Ofrece sala de juntas y acceso a Internet en todas las instalaciones.</t>
-  </si>
-  <si>
-    <t>MXN$ 4,671</t>
-  </si>
-  <si>
-    <t>Hotel Casino Plaza</t>
-  </si>
-  <si>
-    <t>Hotel con facilidades para eventos, ubicado en el centro de la ciudad a escasos minutos de Expo Guadalajara.</t>
-  </si>
-  <si>
-    <t>MXN$ 3,788</t>
-  </si>
-  <si>
-    <t>Hotel Castilla y León</t>
-  </si>
-  <si>
-    <t>Hotel confortable, ubicado a escasos pasos del centro histórico de Guadalajara.</t>
-  </si>
-  <si>
-    <t>MXN$ 1,797</t>
-  </si>
-  <si>
-    <t>Hotel Celta</t>
-  </si>
-  <si>
-    <t>Hotel con piscina, salones de eventos, estacionamiento y acceso a Internet Wi-Fi en todas las áreas. Está cerca de Expo Guadalajara y de un centro comercial.</t>
-  </si>
-  <si>
-    <t>MXN$ 4,481</t>
-  </si>
-  <si>
-    <t>Hotel Cervantes</t>
-  </si>
-  <si>
-    <t>Hotel céntrico y accesible en el distrito colonial de la ciudad, a unas cuadras de la plaza principal y la catedral. Tiene dos salones, restaurante, bar y piscina al aire libre.</t>
-  </si>
-  <si>
-    <t>MXN$ 3,161</t>
-  </si>
-  <si>
     <t>Hotel de Mendoza</t>
   </si>
   <si>
@@ -892,14 +517,322 @@
   </si>
   <si>
     <t>MXN$ 4,484</t>
+  </si>
+  <si>
+    <t>Casa de las Columnas</t>
+  </si>
+  <si>
+    <t>Hermoso y pequeño hotel botique ubicado en el centro de Mérida. Ofrece excelente ubicación y 9 acogedoras habitaciones.</t>
+  </si>
+  <si>
+    <t>MXN$ 5,374</t>
+  </si>
+  <si>
+    <t>Mérida, Yucatán-Zona Centro</t>
+  </si>
+  <si>
+    <t>City Express Mérida</t>
+  </si>
+  <si>
+    <t>Su estupenda ubicación, sus excelentes servicios y las prácticas amenidades, harán de tus días el la Ciudad Blanca, una estancia placentera y provechosa.</t>
+  </si>
+  <si>
+    <t>MXN$ 5,439</t>
+  </si>
+  <si>
+    <t>Mérida, Yucatán-Zona Norte</t>
+  </si>
+  <si>
+    <t>El Conquistador</t>
+  </si>
+  <si>
+    <t>Al hospedarte aquí será una experiencia grata y acogedora, ya que el hotel ofrece diversos servicios y amenidades, además de la conveniencia de estar situado en Paseo Montejo.</t>
+  </si>
+  <si>
+    <t>MXN$ 8,591</t>
+  </si>
+  <si>
+    <t>El Mesón del Marqués</t>
+  </si>
+  <si>
+    <t>Localizado en la calle principal y más bella de la ciudad de Valladolid, te permitirá experimentar la herencia colonial del lugar, mientras disfrutas todo el confort de la propiedad.</t>
+  </si>
+  <si>
+    <t>MXN$ 9,565</t>
+  </si>
+  <si>
+    <t>Valladolid-Yucatán</t>
+  </si>
+  <si>
+    <t>Hacienda Misné</t>
+  </si>
+  <si>
+    <t>Exclusivo hotel estilo hacienda a 13 km del aeropuerto. Cuenta con área ajardinada y salones de eventos.</t>
+  </si>
+  <si>
+    <t>MXN$ 14,089</t>
+  </si>
+  <si>
+    <t>Mérida, Yucatán-Zona Oriente</t>
+  </si>
+  <si>
+    <t>Holiday Inn Express Mérida</t>
+  </si>
+  <si>
+    <t>Hotel de negocios ideal para una estadía llena de comodidades, ya que además de estar bien ubicado, cuenta con una piscina exterior, gimnasio y centro de negocios.</t>
+  </si>
+  <si>
+    <t>MXN$ 7,723</t>
+  </si>
+  <si>
+    <t>Holiday Inn Mérida</t>
+  </si>
+  <si>
+    <t>Pasa una espléndida estancia en las cómodas instalaciones del hotel, con excelentes servicios y la cálida hospitalidad yucateca. Aquí encontrarás una piscina, dos restaurantes y lobby bar.</t>
+  </si>
+  <si>
+    <t>MXN$ 10,602</t>
+  </si>
+  <si>
+    <t>Hotel Boutique Casa San Ángel</t>
+  </si>
+  <si>
+    <t>Tu estadía en este hermoso hotel Sólo Adultos estará llena de encantadores detalles, desde la elegante arquitectura de sus instalaciones hasta los lujosos servicios de tu habitación.</t>
+  </si>
+  <si>
+    <t>MXN$ 12,710</t>
+  </si>
+  <si>
+    <t>Hotel Caribe</t>
+  </si>
+  <si>
+    <t>El hotel es una elección ideal para tus necesidades de hospedaje en la ciudad de Mérida. Excelente servicio y cómodas instalaciones es justo lo que necesita para unas agradables vacaciones.</t>
+  </si>
+  <si>
+    <t>MXN$ 7,900</t>
+  </si>
+  <si>
+    <t>Hotel Colonial</t>
+  </si>
+  <si>
+    <t>El hotel hace honor a su nombre con instalaciones decoradas al estilo colonial mexicano. Aquí encontrarás cómodas habitaciones, una piscina y asoleadero.</t>
+  </si>
+  <si>
+    <t>MXN$ 5,045</t>
+  </si>
+  <si>
+    <t>Hotel del Gobernador</t>
+  </si>
+  <si>
+    <t>Todos los servicios que te ofrece esta propiedad ubicada en Mérida, tienen un magnífico toque de hospitalidad</t>
+  </si>
+  <si>
+    <t>MXN$ 6,670</t>
+  </si>
+  <si>
+    <t>Hotel Eclipse Mérida</t>
+  </si>
+  <si>
+    <t>Ubicado a dos cuadras de la catedral, este hotel está decorado con originales pinturas y ofrece piscina y acceso a Internet inalámbrico en todas las instalaciones.</t>
+  </si>
+  <si>
+    <t>MXN$ 4,824</t>
+  </si>
+  <si>
+    <t>Hotel El Español Paseo de Montejo</t>
+  </si>
+  <si>
+    <t>Confortable hotel a 9 km del aeropuerto, ubicado sobre Paseo de Montejo. Con restaurante y piscina.</t>
+  </si>
+  <si>
+    <t>MXN$ 5,556</t>
+  </si>
+  <si>
+    <t>Hotel Embajadores</t>
+  </si>
+  <si>
+    <t>Hotel con toques modernos y coloniales en el centro histórico, a unas cuadras de la catedral y cerca de distintos parques e iglesias. Tiene piscina, restaurante y Wi-Fi.</t>
+  </si>
+  <si>
+    <t>MXN$ 4,217</t>
+  </si>
+  <si>
+    <t>Hotel Hacienda Inn Aeropuerto</t>
+  </si>
+  <si>
+    <t>Relájate y disfruta tus vacaciones en este apacible hotel de estilo tradicional mexicano, ofrece un buen restaurante y la cercanía al aeropuerto</t>
+  </si>
+  <si>
+    <t>MXN$ 3,814</t>
+  </si>
+  <si>
+    <t>Mérida, Yucatán-Zona Aeropuerto</t>
+  </si>
+  <si>
+    <t>Hotel Maya Yucatán</t>
+  </si>
+  <si>
+    <t>Tus vacaciones se verán impregnadas por la magia de la ciudad de Mérida, ya que al descansar en este hotel gozarás al máximo de cómodos servicios e instalaciones.</t>
+  </si>
+  <si>
+    <t>MXN$ 3,121</t>
+  </si>
+  <si>
+    <t>Hotel Nacional Mérida</t>
+  </si>
+  <si>
+    <t>Un excelente lugar de descanso en Mérida, muy cerca de los mejores atractivos de Mérida y con tarifas accesibles.</t>
+  </si>
+  <si>
+    <t>MXN$ 4,415</t>
+  </si>
+  <si>
+    <t>Hyatt Regency Mérida</t>
+  </si>
+  <si>
+    <t>Goza magníficas instalaciones como una piscina al aire libre, un bien equipado gimnasio, canchas de tenis y divertidas actividades</t>
+  </si>
+  <si>
+    <t>MXN$ 12,727</t>
+  </si>
+  <si>
+    <t>María del Carmen</t>
+  </si>
+  <si>
+    <t>Bello hotel a 7 km del aeropuerto, con piscina, restaurante, bar, salón para eventos y cómodos cuartos.</t>
+  </si>
+  <si>
+    <t>MXN$ 4,163</t>
+  </si>
+  <si>
+    <t>Mesón de la Luna Hotel and Spa</t>
+  </si>
+  <si>
+    <t>Ideal para disfrutar un viaje relajante, cuenta con spa, jacuzzi al are libre, confortables habitaciones y a pocas cuadras de Plaza Altabrisa.</t>
+  </si>
+  <si>
+    <t>MXN$ 7,834</t>
+  </si>
+  <si>
+    <t>Misión Express Mérida Altabrisa</t>
+  </si>
+  <si>
+    <t>Con habitaciones decoradas en un estilo contemporáneo, aquí encontrarás todo lo necesario para desempeñar tus actividades, en especial si viajas por trabajo.</t>
+  </si>
+  <si>
+    <t>MXN$ 4,935</t>
+  </si>
+  <si>
+    <t>Misión Mérida Panamericana</t>
+  </si>
+  <si>
+    <t>Un hotel cuyos orígenes fueron una antigua casona del siglo XIX, que mantiene intacto su espectacular estilo arquitectónico y diseño europeo.</t>
+  </si>
+  <si>
+    <t>MXN$ 5,766</t>
+  </si>
+  <si>
+    <t>Okaan</t>
+  </si>
+  <si>
+    <t>Ubicado dentro de la exuberante selva de Chichén Itzá, aprovecha la energía del lugar en su temazcal, piscina, masajes y cómodas instalaciones.</t>
+  </si>
+  <si>
+    <t>MXN$ 13,983</t>
+  </si>
+  <si>
+    <t>Chichén Itzá-Yucatán</t>
+  </si>
+  <si>
+    <t>Playa Linda Hotel</t>
+  </si>
+  <si>
+    <t>Práctico hotel localizado frente al mar. Ofrece cómodas habitaciones equipadas con prácticos servicios e Internet inalámbrico en cortesía.</t>
+  </si>
+  <si>
+    <t>MXN$ 7,650</t>
+  </si>
+  <si>
+    <t>Progreso-Yucatán</t>
+  </si>
+  <si>
+    <t>Plaza Mirador</t>
+  </si>
+  <si>
+    <t>Este hotel cuenta con cómodas instalaciones para que tu estancia en Mérida sea placentera, entre ellas una piscina, tres salones y restaurante.</t>
+  </si>
+  <si>
+    <t>MXN$ 4,099</t>
+  </si>
+  <si>
+    <t>Posada Toledo and Galería</t>
+  </si>
+  <si>
+    <t>Hotel colonial con Internet WiFi, galería de arte y cuartos climatizados construidos alrededor de un patio central. Se encuentra a dos cuadras de la catedral.</t>
+  </si>
+  <si>
+    <t>MXN$ 5,414</t>
+  </si>
+  <si>
+    <t>Presidente InterContinental Merida</t>
+  </si>
+  <si>
+    <t>Elegante hotel localizado en una de las principales vías de la ciudad, cuenta con modernos servicios, facilidades de negocios y más.</t>
+  </si>
+  <si>
+    <t>MXN$ 57,112</t>
+  </si>
+  <si>
+    <t>Reef Yucatán</t>
+  </si>
+  <si>
+    <t>Además de comodidad, ofrece diversión para adultos y niños, piscina, playa, club de niños, restaurantes, actividades acuáticas, salones para eventos y muchas cosas más.</t>
+  </si>
+  <si>
+    <t>MXN$ 14,150</t>
+  </si>
+  <si>
+    <t>Telchac Puerto</t>
+  </si>
+  <si>
+    <t>Uxmal Resort Maya</t>
+  </si>
+  <si>
+    <t>Confortable hotel en la Ruta Puuc, situado a sólo cinco minutos del sitio arqueológico de Uxmal.</t>
+  </si>
+  <si>
+    <t>MXN$ 6,668</t>
+  </si>
+  <si>
+    <t>Uxmal-Yucatán</t>
+  </si>
+  <si>
+    <t>Wyndham Mérida</t>
+  </si>
+  <si>
+    <t>Lujoso hotel de negocios en una mansión cercana al Paseo de Montejo. Tiene piscina al aire libre, restaurante, bar, gimnasio y espacio para eventos.</t>
+  </si>
+  <si>
+    <t>MXN$ 10,908</t>
+  </si>
+  <si>
+    <t>Xixim Unique Mayan Hotel</t>
+  </si>
+  <si>
+    <t>Bello hotel con atractivas cabañas que tienen buenos servicios para una relajadas vacaciones junto a las playas del Golfo de México, en Celestún.</t>
+  </si>
+  <si>
+    <t>MXN$ 32,251</t>
+  </si>
+  <si>
+    <t>Celestún-Yucatán</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
@@ -934,7 +867,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1248,2142 +1181,2142 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>164</v>
       </c>
       <c r="B2" s="1">
-        <v>2328</v>
+        <v>1074</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>165</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>166</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>168</v>
       </c>
       <c r="B3" s="1">
-        <v>2328</v>
+        <v>1087</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>169</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>168</v>
       </c>
       <c r="B4" s="1">
-        <v>934</v>
+        <v>1087</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>169</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>170</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>172</v>
       </c>
       <c r="B5" s="1">
-        <v>809</v>
+        <v>1718</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>174</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="B6" s="1">
-        <v>728</v>
+        <v>1913</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>176</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>177</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>179</v>
       </c>
       <c r="B7" s="1">
-        <v>1181</v>
+        <v>2817</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>180</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>181</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>183</v>
       </c>
       <c r="B8" s="1">
-        <v>950</v>
+        <v>1544</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>184</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>185</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>183</v>
       </c>
       <c r="B9" s="1">
-        <v>950</v>
+        <v>1544</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>184</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>185</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>186</v>
       </c>
       <c r="B10" s="1">
-        <v>1679</v>
+        <v>2120</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>187</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>188</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>186</v>
       </c>
       <c r="B11" s="1">
-        <v>2081</v>
+        <v>2120</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>187</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="E11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>189</v>
       </c>
       <c r="B12" s="1">
-        <v>1375</v>
+        <v>2542</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>190</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>191</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>192</v>
       </c>
       <c r="B13" s="1">
-        <v>978</v>
+        <v>1580</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>193</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>194</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>41</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>195</v>
       </c>
       <c r="B14" s="1">
-        <v>1441</v>
+        <v>1009</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>196</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>197</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>195</v>
       </c>
       <c r="B15" s="1">
-        <v>1435</v>
+        <v>1009</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>196</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>197</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>198</v>
       </c>
       <c r="B16" s="1">
-        <v>1053</v>
+        <v>1334</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>199</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="E16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>201</v>
       </c>
       <c r="B17" s="1">
-        <v>1309</v>
+        <v>964</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>202</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>203</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>25</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>204</v>
       </c>
       <c r="B18" s="1">
-        <v>2566</v>
+        <v>1111</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>205</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>206</v>
       </c>
       <c r="E18" t="s">
         <v>6</v>
       </c>
       <c r="F18" t="s">
-        <v>41</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>204</v>
       </c>
       <c r="B19" s="1">
-        <v>2566</v>
+        <v>1111</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>205</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>206</v>
       </c>
       <c r="E19" t="s">
         <v>6</v>
       </c>
       <c r="F19" t="s">
-        <v>41</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>207</v>
       </c>
       <c r="B20" s="1">
-        <v>1820</v>
+        <v>843</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>208</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>209</v>
       </c>
       <c r="E20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>210</v>
       </c>
       <c r="B21" s="1">
-        <v>646</v>
+        <v>762</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>211</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>212</v>
       </c>
       <c r="E21" t="s">
         <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>25</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>210</v>
       </c>
       <c r="B22" s="1">
-        <v>646</v>
+        <v>762</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>211</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>212</v>
       </c>
       <c r="E22" t="s">
         <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>25</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>214</v>
       </c>
       <c r="B23" s="1">
-        <v>449</v>
+        <v>624</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>215</v>
       </c>
       <c r="D23" t="s">
-        <v>65</v>
+        <v>216</v>
       </c>
       <c r="E23" t="s">
         <v>6</v>
       </c>
       <c r="F23" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>214</v>
       </c>
       <c r="B24" s="1">
-        <v>1345</v>
+        <v>624</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>215</v>
       </c>
       <c r="D24" t="s">
-        <v>68</v>
+        <v>216</v>
       </c>
       <c r="E24" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F24" t="s">
-        <v>25</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>217</v>
       </c>
       <c r="B25" s="1">
-        <v>2327</v>
+        <v>883</v>
       </c>
       <c r="C25" t="s">
-        <v>70</v>
+        <v>218</v>
       </c>
       <c r="D25" t="s">
-        <v>71</v>
+        <v>219</v>
       </c>
       <c r="E25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>217</v>
       </c>
       <c r="B26" s="1">
-        <v>1601</v>
+        <v>883</v>
       </c>
       <c r="C26" t="s">
-        <v>73</v>
+        <v>218</v>
       </c>
       <c r="D26" t="s">
-        <v>74</v>
+        <v>219</v>
       </c>
       <c r="E26" t="s">
         <v>6</v>
       </c>
       <c r="F26" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>220</v>
       </c>
       <c r="B27" s="1">
-        <v>2567</v>
+        <v>2545</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>221</v>
       </c>
       <c r="D27" t="s">
-        <v>77</v>
+        <v>222</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F27" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>220</v>
       </c>
       <c r="B28" s="1">
-        <v>1106</v>
+        <v>2545</v>
       </c>
       <c r="C28" t="s">
-        <v>79</v>
+        <v>221</v>
       </c>
       <c r="D28" t="s">
-        <v>80</v>
+        <v>222</v>
       </c>
       <c r="E28" t="s">
         <v>7</v>
       </c>
       <c r="F28" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>223</v>
       </c>
       <c r="B29" s="1">
-        <v>1269</v>
+        <v>832</v>
       </c>
       <c r="C29" t="s">
-        <v>82</v>
+        <v>224</v>
       </c>
       <c r="D29" t="s">
-        <v>83</v>
+        <v>225</v>
       </c>
       <c r="E29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F29" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>223</v>
       </c>
       <c r="B30" s="1">
-        <v>2584</v>
+        <v>832</v>
       </c>
       <c r="C30" t="s">
-        <v>85</v>
+        <v>224</v>
       </c>
       <c r="D30" t="s">
-        <v>86</v>
+        <v>225</v>
       </c>
       <c r="E30" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F30" t="s">
-        <v>87</v>
+        <v>167</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>88</v>
+        <v>226</v>
       </c>
       <c r="B31" s="1">
-        <v>1785</v>
+        <v>1566</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>227</v>
       </c>
       <c r="D31" t="s">
-        <v>90</v>
+        <v>228</v>
       </c>
       <c r="E31" t="s">
         <v>7</v>
       </c>
       <c r="F31" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>91</v>
+        <v>229</v>
       </c>
       <c r="B32" s="1">
-        <v>1972</v>
+        <v>987</v>
       </c>
       <c r="C32" t="s">
-        <v>92</v>
+        <v>230</v>
       </c>
       <c r="D32" t="s">
-        <v>93</v>
+        <v>231</v>
       </c>
       <c r="E32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>94</v>
+        <v>229</v>
       </c>
       <c r="B33" s="1">
-        <v>1766</v>
+        <v>987</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>230</v>
       </c>
       <c r="D33" t="s">
-        <v>96</v>
+        <v>231</v>
       </c>
       <c r="E33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F33" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>97</v>
+        <v>232</v>
       </c>
       <c r="B34" s="1">
-        <v>1460</v>
+        <v>1153</v>
       </c>
       <c r="C34" t="s">
-        <v>98</v>
+        <v>233</v>
       </c>
       <c r="D34" t="s">
-        <v>99</v>
+        <v>234</v>
       </c>
       <c r="E34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F34" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>97</v>
+        <v>232</v>
       </c>
       <c r="B35" s="1">
-        <v>1460</v>
+        <v>1153</v>
       </c>
       <c r="C35" t="s">
-        <v>98</v>
+        <v>233</v>
       </c>
       <c r="D35" t="s">
-        <v>99</v>
+        <v>234</v>
       </c>
       <c r="E35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>100</v>
+        <v>235</v>
       </c>
       <c r="B36" s="1">
-        <v>1506</v>
+        <v>2796</v>
       </c>
       <c r="C36" t="s">
-        <v>101</v>
+        <v>236</v>
       </c>
       <c r="D36" t="s">
-        <v>102</v>
+        <v>237</v>
       </c>
       <c r="E36" t="s">
         <v>7</v>
       </c>
       <c r="F36" t="s">
-        <v>12</v>
+        <v>238</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>103</v>
+        <v>239</v>
       </c>
       <c r="B37" s="1">
-        <v>1724</v>
+        <v>1530</v>
       </c>
       <c r="C37" t="s">
-        <v>104</v>
+        <v>240</v>
       </c>
       <c r="D37" t="s">
-        <v>105</v>
+        <v>241</v>
       </c>
       <c r="E37" t="s">
         <v>7</v>
       </c>
       <c r="F37" t="s">
-        <v>12</v>
+        <v>242</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>106</v>
+        <v>239</v>
       </c>
       <c r="B38" s="1">
-        <v>1804</v>
+        <v>1530</v>
       </c>
       <c r="C38" t="s">
-        <v>107</v>
+        <v>240</v>
       </c>
       <c r="D38" t="s">
-        <v>108</v>
+        <v>241</v>
       </c>
       <c r="E38" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F38" t="s">
-        <v>25</v>
+        <v>242</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>106</v>
+        <v>243</v>
       </c>
       <c r="B39" s="1">
-        <v>1804</v>
+        <v>819</v>
       </c>
       <c r="C39" t="s">
-        <v>107</v>
+        <v>244</v>
       </c>
       <c r="D39" t="s">
-        <v>108</v>
+        <v>245</v>
       </c>
       <c r="E39" t="s">
         <v>6</v>
       </c>
       <c r="F39" t="s">
-        <v>25</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>109</v>
+        <v>243</v>
       </c>
       <c r="B40" s="1">
-        <v>1645</v>
+        <v>819</v>
       </c>
       <c r="C40" t="s">
-        <v>110</v>
+        <v>244</v>
       </c>
       <c r="D40" t="s">
-        <v>111</v>
+        <v>245</v>
       </c>
       <c r="E40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>112</v>
+        <v>246</v>
       </c>
       <c r="B41" s="1">
-        <v>1723</v>
+        <v>1082</v>
       </c>
       <c r="C41" t="s">
-        <v>113</v>
+        <v>247</v>
       </c>
       <c r="D41" t="s">
-        <v>114</v>
+        <v>248</v>
       </c>
       <c r="E41" t="s">
         <v>6</v>
       </c>
       <c r="F41" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>115</v>
+        <v>249</v>
       </c>
       <c r="B42" s="1">
-        <v>1113</v>
+        <v>11422</v>
       </c>
       <c r="C42" t="s">
-        <v>116</v>
+        <v>250</v>
       </c>
       <c r="D42" t="s">
-        <v>117</v>
+        <v>251</v>
       </c>
       <c r="E42" t="s">
         <v>7</v>
       </c>
       <c r="F42" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>118</v>
+        <v>249</v>
       </c>
       <c r="B43" s="1">
-        <v>628</v>
+        <v>11422</v>
       </c>
       <c r="C43" t="s">
-        <v>119</v>
+        <v>250</v>
       </c>
       <c r="D43" t="s">
-        <v>120</v>
+        <v>251</v>
       </c>
       <c r="E43" t="s">
         <v>7</v>
       </c>
       <c r="F43" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>121</v>
+        <v>252</v>
       </c>
       <c r="B44" s="1">
-        <v>934</v>
+        <v>2830</v>
       </c>
       <c r="C44" t="s">
-        <v>122</v>
+        <v>253</v>
       </c>
       <c r="D44" t="s">
-        <v>123</v>
+        <v>254</v>
       </c>
       <c r="E44" t="s">
         <v>6</v>
       </c>
       <c r="F44" t="s">
-        <v>25</v>
+        <v>255</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>124</v>
+        <v>252</v>
       </c>
       <c r="B45" s="1">
-        <v>757</v>
+        <v>2830</v>
       </c>
       <c r="C45" t="s">
-        <v>125</v>
+        <v>253</v>
       </c>
       <c r="D45" t="s">
-        <v>126</v>
+        <v>254</v>
       </c>
       <c r="E45" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F45" t="s">
-        <v>12</v>
+        <v>255</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>127</v>
+        <v>256</v>
       </c>
       <c r="B46" s="1">
-        <v>359</v>
+        <v>1333</v>
       </c>
       <c r="C46" t="s">
-        <v>128</v>
+        <v>257</v>
       </c>
       <c r="D46" t="s">
-        <v>129</v>
+        <v>258</v>
       </c>
       <c r="E46" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F46" t="s">
-        <v>12</v>
+        <v>259</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>130</v>
+        <v>260</v>
       </c>
       <c r="B47" s="1">
-        <v>896</v>
+        <v>2181</v>
       </c>
       <c r="C47" t="s">
-        <v>131</v>
+        <v>261</v>
       </c>
       <c r="D47" t="s">
-        <v>132</v>
+        <v>262</v>
       </c>
       <c r="E47" t="s">
         <v>7</v>
       </c>
       <c r="F47" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>130</v>
+        <v>260</v>
       </c>
       <c r="B48" s="1">
-        <v>896</v>
+        <v>2181</v>
       </c>
       <c r="C48" t="s">
-        <v>131</v>
+        <v>261</v>
       </c>
       <c r="D48" t="s">
-        <v>132</v>
+        <v>262</v>
       </c>
       <c r="E48" t="s">
         <v>7</v>
       </c>
       <c r="F48" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>133</v>
+        <v>263</v>
       </c>
       <c r="B49" s="1">
-        <v>632</v>
+        <v>6450</v>
       </c>
       <c r="C49" t="s">
-        <v>134</v>
+        <v>264</v>
       </c>
       <c r="D49" t="s">
-        <v>135</v>
+        <v>265</v>
       </c>
       <c r="E49" t="s">
         <v>6</v>
       </c>
       <c r="F49" t="s">
-        <v>12</v>
+        <v>266</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>136</v>
+        <v>11</v>
       </c>
       <c r="B50" s="2">
         <v>1086</v>
       </c>
       <c r="C50" t="s">
-        <v>137</v>
+        <v>12</v>
       </c>
       <c r="D50" t="s">
-        <v>138</v>
+        <v>13</v>
       </c>
       <c r="E50" t="s">
         <v>7</v>
       </c>
       <c r="F50" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>139</v>
+        <v>14</v>
       </c>
       <c r="B51" s="2">
         <v>1187</v>
       </c>
       <c r="C51" t="s">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="D51" t="s">
-        <v>141</v>
+        <v>16</v>
       </c>
       <c r="E51" t="s">
         <v>6</v>
       </c>
       <c r="F51" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>142</v>
+        <v>17</v>
       </c>
       <c r="B52" s="2">
         <v>1000</v>
       </c>
       <c r="C52" t="s">
-        <v>143</v>
+        <v>18</v>
       </c>
       <c r="D52" t="s">
-        <v>144</v>
+        <v>19</v>
       </c>
       <c r="E52" t="s">
         <v>6</v>
       </c>
       <c r="F52" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>145</v>
+        <v>20</v>
       </c>
       <c r="B53" s="2">
         <v>710</v>
       </c>
       <c r="C53" t="s">
-        <v>146</v>
+        <v>21</v>
       </c>
       <c r="D53" t="s">
-        <v>147</v>
+        <v>22</v>
       </c>
       <c r="E53" t="s">
         <v>7</v>
       </c>
       <c r="F53" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>148</v>
+        <v>23</v>
       </c>
       <c r="B54" s="2">
         <v>747</v>
       </c>
       <c r="C54" t="s">
-        <v>149</v>
+        <v>24</v>
       </c>
       <c r="D54" t="s">
-        <v>150</v>
+        <v>25</v>
       </c>
       <c r="E54" t="s">
         <v>6</v>
       </c>
       <c r="F54" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>151</v>
+        <v>26</v>
       </c>
       <c r="B55" s="2">
         <v>949</v>
       </c>
       <c r="C55" t="s">
-        <v>152</v>
+        <v>27</v>
       </c>
       <c r="D55" t="s">
-        <v>153</v>
+        <v>28</v>
       </c>
       <c r="E55" t="s">
         <v>6</v>
       </c>
       <c r="F55" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>154</v>
+        <v>29</v>
       </c>
       <c r="B56" s="2">
         <v>810</v>
       </c>
       <c r="C56" t="s">
-        <v>155</v>
+        <v>30</v>
       </c>
       <c r="D56" t="s">
-        <v>156</v>
+        <v>31</v>
       </c>
       <c r="E56" t="s">
         <v>6</v>
       </c>
       <c r="F56" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>157</v>
+        <v>32</v>
       </c>
       <c r="B57" s="2">
         <v>946</v>
       </c>
       <c r="C57" t="s">
-        <v>158</v>
+        <v>33</v>
       </c>
       <c r="D57" t="s">
-        <v>159</v>
+        <v>34</v>
       </c>
       <c r="E57" t="s">
         <v>6</v>
       </c>
       <c r="F57" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>160</v>
+        <v>35</v>
       </c>
       <c r="B58" s="2">
         <v>1631</v>
       </c>
       <c r="C58" t="s">
-        <v>161</v>
+        <v>36</v>
       </c>
       <c r="D58" t="s">
-        <v>162</v>
+        <v>37</v>
       </c>
       <c r="E58" t="s">
         <v>6</v>
       </c>
       <c r="F58" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>163</v>
+        <v>38</v>
       </c>
       <c r="B59" s="2">
         <v>712</v>
       </c>
       <c r="C59" t="s">
-        <v>164</v>
+        <v>39</v>
       </c>
       <c r="D59" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="E59" t="s">
         <v>7</v>
       </c>
       <c r="F59" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>163</v>
+        <v>38</v>
       </c>
       <c r="B60" s="2">
         <v>712</v>
       </c>
       <c r="C60" t="s">
-        <v>164</v>
+        <v>39</v>
       </c>
       <c r="D60" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="E60" t="s">
         <v>7</v>
       </c>
       <c r="F60" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>166</v>
+        <v>41</v>
       </c>
       <c r="B61" s="2">
         <v>877</v>
       </c>
       <c r="C61" t="s">
-        <v>167</v>
+        <v>42</v>
       </c>
       <c r="D61" t="s">
-        <v>168</v>
+        <v>43</v>
       </c>
       <c r="E61" t="s">
         <v>8</v>
       </c>
       <c r="F61" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>169</v>
+        <v>44</v>
       </c>
       <c r="B62" s="2">
         <v>636</v>
       </c>
       <c r="C62" t="s">
-        <v>170</v>
+        <v>45</v>
       </c>
       <c r="D62" t="s">
-        <v>171</v>
+        <v>46</v>
       </c>
       <c r="E62" t="s">
         <v>6</v>
       </c>
       <c r="F62" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>172</v>
+        <v>47</v>
       </c>
       <c r="B63" s="2">
         <v>794</v>
       </c>
       <c r="C63" t="s">
-        <v>173</v>
+        <v>48</v>
       </c>
       <c r="D63" t="s">
-        <v>174</v>
+        <v>49</v>
       </c>
       <c r="E63" t="s">
         <v>6</v>
       </c>
       <c r="F63" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>175</v>
+        <v>50</v>
       </c>
       <c r="B64" s="2">
         <v>1086</v>
       </c>
       <c r="C64" t="s">
-        <v>176</v>
+        <v>51</v>
       </c>
       <c r="D64" t="s">
-        <v>177</v>
+        <v>52</v>
       </c>
       <c r="E64" t="s">
         <v>8</v>
       </c>
       <c r="F64" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>175</v>
+        <v>50</v>
       </c>
       <c r="B65" s="2">
         <v>1086</v>
       </c>
       <c r="C65" t="s">
-        <v>176</v>
+        <v>51</v>
       </c>
       <c r="D65" t="s">
-        <v>177</v>
+        <v>52</v>
       </c>
       <c r="E65" t="s">
         <v>8</v>
       </c>
       <c r="F65" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>178</v>
+        <v>53</v>
       </c>
       <c r="B66" s="2">
         <v>1132</v>
       </c>
       <c r="C66" t="s">
-        <v>179</v>
+        <v>54</v>
       </c>
       <c r="D66" t="s">
-        <v>180</v>
+        <v>55</v>
       </c>
       <c r="E66" t="s">
         <v>7</v>
       </c>
       <c r="F66" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>181</v>
+        <v>56</v>
       </c>
       <c r="B67" s="2">
         <v>1208</v>
       </c>
       <c r="C67" t="s">
-        <v>182</v>
+        <v>57</v>
       </c>
       <c r="D67" t="s">
-        <v>183</v>
+        <v>58</v>
       </c>
       <c r="E67" t="s">
         <v>6</v>
       </c>
       <c r="F67" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>184</v>
+        <v>59</v>
       </c>
       <c r="B68" s="2">
         <v>930</v>
       </c>
       <c r="C68" t="s">
-        <v>185</v>
+        <v>60</v>
       </c>
       <c r="D68" t="s">
-        <v>186</v>
+        <v>61</v>
       </c>
       <c r="E68" t="s">
         <v>6</v>
       </c>
       <c r="F68" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>187</v>
+        <v>62</v>
       </c>
       <c r="B69" s="2">
         <v>607</v>
       </c>
       <c r="C69" t="s">
-        <v>188</v>
+        <v>63</v>
       </c>
       <c r="D69" t="s">
-        <v>189</v>
+        <v>64</v>
       </c>
       <c r="E69" t="s">
         <v>6</v>
       </c>
       <c r="F69" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>190</v>
+        <v>65</v>
       </c>
       <c r="B70" s="2">
         <v>1560</v>
       </c>
       <c r="C70" t="s">
-        <v>191</v>
+        <v>66</v>
       </c>
       <c r="D70" t="s">
-        <v>192</v>
+        <v>67</v>
       </c>
       <c r="E70" t="s">
         <v>7</v>
       </c>
       <c r="F70" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>193</v>
+        <v>68</v>
       </c>
       <c r="B71" s="2">
         <v>853</v>
       </c>
       <c r="C71" t="s">
-        <v>194</v>
+        <v>69</v>
       </c>
       <c r="D71" t="s">
-        <v>195</v>
+        <v>70</v>
       </c>
       <c r="E71" t="s">
         <v>6</v>
       </c>
       <c r="F71" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>196</v>
+        <v>71</v>
       </c>
       <c r="B72" s="2">
         <v>2784</v>
       </c>
       <c r="C72" t="s">
-        <v>197</v>
+        <v>72</v>
       </c>
       <c r="D72" t="s">
-        <v>198</v>
+        <v>73</v>
       </c>
       <c r="E72" t="s">
         <v>7</v>
       </c>
       <c r="F72" t="s">
-        <v>199</v>
+        <v>74</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>200</v>
+        <v>75</v>
       </c>
       <c r="B73" s="2">
         <v>611</v>
       </c>
       <c r="C73" t="s">
-        <v>201</v>
+        <v>76</v>
       </c>
       <c r="D73" t="s">
-        <v>202</v>
+        <v>77</v>
       </c>
       <c r="E73" t="s">
         <v>6</v>
       </c>
       <c r="F73" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>203</v>
+        <v>78</v>
       </c>
       <c r="B74" s="2">
         <v>5824</v>
       </c>
       <c r="C74" t="s">
-        <v>204</v>
+        <v>79</v>
       </c>
       <c r="D74" t="s">
-        <v>205</v>
+        <v>80</v>
       </c>
       <c r="E74" t="s">
         <v>8</v>
       </c>
       <c r="F74" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>206</v>
+        <v>81</v>
       </c>
       <c r="B75" s="2">
         <v>1611</v>
       </c>
       <c r="C75" t="s">
-        <v>207</v>
+        <v>82</v>
       </c>
       <c r="D75" t="s">
-        <v>208</v>
+        <v>83</v>
       </c>
       <c r="E75" t="s">
         <v>7</v>
       </c>
       <c r="F75" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>206</v>
+        <v>81</v>
       </c>
       <c r="B76" s="2">
         <v>1611</v>
       </c>
       <c r="C76" t="s">
-        <v>207</v>
+        <v>82</v>
       </c>
       <c r="D76" t="s">
-        <v>208</v>
+        <v>83</v>
       </c>
       <c r="E76" t="s">
         <v>7</v>
       </c>
       <c r="F76" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>209</v>
+        <v>84</v>
       </c>
       <c r="B77" s="2">
         <v>1360</v>
       </c>
       <c r="C77" t="s">
-        <v>210</v>
+        <v>85</v>
       </c>
       <c r="D77" t="s">
-        <v>211</v>
+        <v>86</v>
       </c>
       <c r="E77" t="s">
         <v>7</v>
       </c>
       <c r="F77" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>212</v>
+        <v>87</v>
       </c>
       <c r="B78" s="2">
         <v>987</v>
       </c>
       <c r="C78" t="s">
-        <v>213</v>
+        <v>88</v>
       </c>
       <c r="D78" t="s">
-        <v>214</v>
+        <v>89</v>
       </c>
       <c r="E78" t="s">
         <v>6</v>
       </c>
       <c r="F78" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>215</v>
+        <v>90</v>
       </c>
       <c r="B79" s="2">
         <v>1343</v>
       </c>
       <c r="C79" t="s">
-        <v>216</v>
+        <v>91</v>
       </c>
       <c r="D79" t="s">
-        <v>217</v>
+        <v>92</v>
       </c>
       <c r="E79" t="s">
         <v>7</v>
       </c>
       <c r="F79" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>218</v>
+        <v>93</v>
       </c>
       <c r="B80" s="2">
         <v>1187</v>
       </c>
       <c r="C80" t="s">
-        <v>219</v>
+        <v>94</v>
       </c>
       <c r="D80" t="s">
-        <v>220</v>
+        <v>95</v>
       </c>
       <c r="E80" t="s">
         <v>7</v>
       </c>
       <c r="F80" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>221</v>
+        <v>96</v>
       </c>
       <c r="B81" s="2">
         <v>1232</v>
       </c>
       <c r="C81" t="s">
-        <v>222</v>
+        <v>97</v>
       </c>
       <c r="D81" t="s">
-        <v>223</v>
+        <v>98</v>
       </c>
       <c r="E81" t="s">
         <v>7</v>
       </c>
       <c r="F81" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>221</v>
+        <v>96</v>
       </c>
       <c r="B82" s="2">
         <v>1232</v>
       </c>
       <c r="C82" t="s">
-        <v>222</v>
+        <v>97</v>
       </c>
       <c r="D82" t="s">
-        <v>223</v>
+        <v>98</v>
       </c>
       <c r="E82" t="s">
         <v>7</v>
       </c>
       <c r="F82" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>224</v>
+        <v>99</v>
       </c>
       <c r="B83" s="2">
         <v>1152</v>
       </c>
       <c r="C83" t="s">
-        <v>225</v>
+        <v>100</v>
       </c>
       <c r="D83" t="s">
-        <v>226</v>
+        <v>101</v>
       </c>
       <c r="E83" t="s">
         <v>7</v>
       </c>
       <c r="F83" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>227</v>
+        <v>102</v>
       </c>
       <c r="B84" s="2">
         <v>1027</v>
       </c>
       <c r="C84" t="s">
-        <v>228</v>
+        <v>103</v>
       </c>
       <c r="D84" t="s">
-        <v>229</v>
+        <v>104</v>
       </c>
       <c r="E84" t="s">
         <v>6</v>
       </c>
       <c r="F84" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>230</v>
+        <v>105</v>
       </c>
       <c r="B85" s="2">
         <v>1084</v>
       </c>
       <c r="C85" t="s">
-        <v>231</v>
+        <v>106</v>
       </c>
       <c r="D85" t="s">
-        <v>232</v>
+        <v>107</v>
       </c>
       <c r="E85" t="s">
         <v>6</v>
       </c>
       <c r="F85" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>233</v>
+        <v>108</v>
       </c>
       <c r="B86" s="2">
         <v>917</v>
       </c>
       <c r="C86" t="s">
-        <v>234</v>
+        <v>109</v>
       </c>
       <c r="D86" t="s">
-        <v>235</v>
+        <v>110</v>
       </c>
       <c r="E86" t="s">
         <v>7</v>
       </c>
       <c r="F86" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>233</v>
+        <v>108</v>
       </c>
       <c r="B87" s="2">
         <v>917</v>
       </c>
       <c r="C87" t="s">
-        <v>234</v>
+        <v>109</v>
       </c>
       <c r="D87" t="s">
-        <v>235</v>
+        <v>110</v>
       </c>
       <c r="E87" t="s">
         <v>7</v>
       </c>
       <c r="F87" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>236</v>
+        <v>111</v>
       </c>
       <c r="B88" s="2">
         <v>606</v>
       </c>
       <c r="C88" t="s">
-        <v>237</v>
+        <v>112</v>
       </c>
       <c r="D88" t="s">
-        <v>238</v>
+        <v>113</v>
       </c>
       <c r="E88" t="s">
         <v>6</v>
       </c>
       <c r="F88" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>236</v>
+        <v>111</v>
       </c>
       <c r="B89" s="2">
         <v>606</v>
       </c>
       <c r="C89" t="s">
-        <v>237</v>
+        <v>112</v>
       </c>
       <c r="D89" t="s">
-        <v>238</v>
+        <v>113</v>
       </c>
       <c r="E89" t="s">
         <v>6</v>
       </c>
       <c r="F89" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>239</v>
+        <v>114</v>
       </c>
       <c r="B90" s="2">
         <v>1489</v>
       </c>
       <c r="C90" t="s">
-        <v>240</v>
+        <v>115</v>
       </c>
       <c r="D90" t="s">
-        <v>241</v>
+        <v>116</v>
       </c>
       <c r="E90" t="s">
         <v>7</v>
       </c>
       <c r="F90" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>239</v>
+        <v>114</v>
       </c>
       <c r="B91" s="2">
         <v>1489</v>
       </c>
       <c r="C91" t="s">
-        <v>240</v>
+        <v>115</v>
       </c>
       <c r="D91" t="s">
-        <v>241</v>
+        <v>116</v>
       </c>
       <c r="E91" t="s">
         <v>7</v>
       </c>
       <c r="F91" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>242</v>
+        <v>117</v>
       </c>
       <c r="B92" s="2">
         <v>737</v>
       </c>
       <c r="C92" t="s">
-        <v>243</v>
+        <v>118</v>
       </c>
       <c r="D92" t="s">
-        <v>244</v>
+        <v>119</v>
       </c>
       <c r="E92" t="s">
         <v>7</v>
       </c>
       <c r="F92" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>245</v>
+        <v>120</v>
       </c>
       <c r="B93" s="2">
         <v>2618</v>
       </c>
       <c r="C93" t="s">
-        <v>246</v>
+        <v>121</v>
       </c>
       <c r="D93" t="s">
-        <v>247</v>
+        <v>122</v>
       </c>
       <c r="E93" t="s">
         <v>7</v>
       </c>
       <c r="F93" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>248</v>
+        <v>123</v>
       </c>
       <c r="B94" s="2">
         <v>1694</v>
       </c>
       <c r="C94" t="s">
-        <v>249</v>
+        <v>124</v>
       </c>
       <c r="D94" t="s">
-        <v>250</v>
+        <v>125</v>
       </c>
       <c r="E94" t="s">
         <v>6</v>
       </c>
       <c r="F94" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>251</v>
+        <v>126</v>
       </c>
       <c r="B95" s="2">
         <v>1663</v>
       </c>
       <c r="C95" t="s">
-        <v>252</v>
+        <v>127</v>
       </c>
       <c r="D95" t="s">
-        <v>253</v>
+        <v>128</v>
       </c>
       <c r="E95" t="s">
         <v>8</v>
       </c>
       <c r="F95" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>251</v>
+        <v>126</v>
       </c>
       <c r="B96" s="2">
         <v>1663</v>
       </c>
       <c r="C96" t="s">
-        <v>252</v>
+        <v>127</v>
       </c>
       <c r="D96" t="s">
-        <v>253</v>
+        <v>128</v>
       </c>
       <c r="E96" t="s">
         <v>8</v>
       </c>
       <c r="F96" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>254</v>
+        <v>129</v>
       </c>
       <c r="B97" s="2">
         <v>662</v>
       </c>
       <c r="C97" t="s">
-        <v>255</v>
+        <v>130</v>
       </c>
       <c r="D97" t="s">
-        <v>256</v>
+        <v>131</v>
       </c>
       <c r="E97" t="s">
         <v>6</v>
       </c>
       <c r="F97" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>257</v>
+        <v>132</v>
       </c>
       <c r="B98" s="2">
         <v>5817</v>
       </c>
       <c r="C98" t="s">
-        <v>258</v>
+        <v>133</v>
       </c>
       <c r="D98" t="s">
-        <v>259</v>
+        <v>134</v>
       </c>
       <c r="E98" t="s">
         <v>7</v>
       </c>
       <c r="F98" t="s">
-        <v>260</v>
+        <v>135</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>261</v>
+        <v>136</v>
       </c>
       <c r="B99" s="2">
         <v>806</v>
       </c>
       <c r="C99" t="s">
-        <v>262</v>
+        <v>137</v>
       </c>
       <c r="D99" t="s">
-        <v>263</v>
+        <v>138</v>
       </c>
       <c r="E99" t="s">
         <v>7</v>
       </c>
       <c r="F99" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>264</v>
+        <v>139</v>
       </c>
       <c r="B100" s="2">
         <v>1784</v>
       </c>
       <c r="C100" t="s">
-        <v>265</v>
+        <v>140</v>
       </c>
       <c r="D100" t="s">
-        <v>266</v>
+        <v>141</v>
       </c>
       <c r="E100" t="s">
         <v>8</v>
       </c>
       <c r="F100" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>267</v>
+        <v>142</v>
       </c>
       <c r="B101" s="2">
         <v>581</v>
       </c>
       <c r="C101" t="s">
-        <v>268</v>
+        <v>143</v>
       </c>
       <c r="D101" t="s">
-        <v>269</v>
+        <v>144</v>
       </c>
       <c r="E101" t="s">
         <v>6</v>
       </c>
       <c r="F101" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>270</v>
+        <v>145</v>
       </c>
       <c r="B102" s="2">
         <v>12331</v>
       </c>
       <c r="C102" t="s">
-        <v>271</v>
+        <v>146</v>
       </c>
       <c r="D102" t="s">
-        <v>272</v>
+        <v>147</v>
       </c>
       <c r="E102" t="s">
         <v>7</v>
       </c>
       <c r="F102" t="s">
-        <v>273</v>
+        <v>148</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>274</v>
+        <v>149</v>
       </c>
       <c r="B103" s="2">
         <v>1428</v>
       </c>
       <c r="C103" t="s">
-        <v>275</v>
+        <v>150</v>
       </c>
       <c r="D103" t="s">
-        <v>276</v>
+        <v>151</v>
       </c>
       <c r="E103" t="s">
         <v>7</v>
       </c>
       <c r="F103" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>277</v>
+        <v>152</v>
       </c>
       <c r="B104" s="2">
         <v>11539</v>
       </c>
       <c r="C104" t="s">
-        <v>278</v>
+        <v>153</v>
       </c>
       <c r="D104" t="s">
-        <v>279</v>
+        <v>154</v>
       </c>
       <c r="E104" t="s">
         <v>8</v>
       </c>
       <c r="F104" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>280</v>
+        <v>155</v>
       </c>
       <c r="B105" s="2">
         <v>1678</v>
       </c>
       <c r="C105" t="s">
-        <v>281</v>
+        <v>156</v>
       </c>
       <c r="D105" t="s">
-        <v>282</v>
+        <v>157</v>
       </c>
       <c r="E105" t="s">
         <v>6</v>
       </c>
       <c r="F105" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>280</v>
+        <v>155</v>
       </c>
       <c r="B106" s="2">
         <v>1678</v>
       </c>
       <c r="C106" t="s">
-        <v>281</v>
+        <v>156</v>
       </c>
       <c r="D106" t="s">
-        <v>282</v>
+        <v>157</v>
       </c>
       <c r="E106" t="s">
         <v>6</v>
       </c>
       <c r="F106" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>283</v>
+        <v>158</v>
       </c>
       <c r="B107" s="2">
         <v>1255</v>
       </c>
       <c r="C107" t="s">
-        <v>284</v>
+        <v>159</v>
       </c>
       <c r="D107" t="s">
-        <v>285</v>
+        <v>160</v>
       </c>
       <c r="E107" t="s">
         <v>6</v>
       </c>
       <c r="F107" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>286</v>
+        <v>161</v>
       </c>
       <c r="B108" s="2">
         <v>896</v>
       </c>
       <c r="C108" t="s">
-        <v>287</v>
+        <v>162</v>
       </c>
       <c r="D108" t="s">
-        <v>288</v>
+        <v>163</v>
       </c>
       <c r="E108" t="s">
         <v>6</v>
       </c>
       <c r="F108" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>